<commit_message>
actualizacion del doc 7/5
tareas reordenadas y tablas y tareas de empresas puestas
</commit_message>
<xml_diff>
--- a/Documentos/Tiempos x Recurso x Sprint (6+1 Software).xlsx
+++ b/Documentos/Tiempos x Recurso x Sprint (6+1 Software).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uni\LAB SOFT\TP-MASTER SECURITY SYSTEM\Entregas\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uni\LAB SOFT\TP-MASTER SECURITY SYSTEM\Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBA42AA-3571-44BF-BB97-6F33685C109C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A31AB7E-4E3A-42E9-AECD-D276B3FB8E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="18192" windowHeight="9852" xr2:uid="{2AAAEB99-6391-463B-8E85-5B11966A4D20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AAAEB99-6391-463B-8E85-5B11966A4D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -894,19 +894,19 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>36</c:v>
@@ -1042,19 +1042,19 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>47</c:v>
@@ -1190,7 +1190,7 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>23</c:v>
@@ -2520,7 +2520,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2592,20 +2592,20 @@
         <v>54</v>
       </c>
       <c r="D3" s="2">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2">
         <v>15</v>
       </c>
       <c r="H3" s="13">
         <f t="shared" si="0"/>
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -2616,10 +2616,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="2">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E4" s="2">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2">
         <v>23</v>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="H4" s="13">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2640,10 +2640,10 @@
         <v>52</v>
       </c>
       <c r="D5" s="2">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E5" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F5" s="2">
         <v>32</v>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="H5" s="13">
         <f t="shared" si="0"/>
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -2688,10 +2688,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E7" s="2">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2">
         <v>30</v>
@@ -2738,15 +2738,15 @@
       </c>
       <c r="D9" s="15">
         <f>SUM(D2:D8)</f>
-        <v>314</v>
+        <v>380</v>
       </c>
       <c r="E9" s="15">
         <f>SUM(E2:E8)</f>
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="F9" s="15">
         <f>SUM(F2:F8)</f>
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="G9" s="15">
         <f>SUM(G2:G8)</f>
@@ -2754,7 +2754,7 @@
       </c>
       <c r="H9" s="16">
         <f t="shared" si="0"/>
-        <v>1211</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -2874,15 +2874,15 @@
         <v>50</v>
       </c>
       <c r="E21" s="2">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2">
@@ -2891,7 +2891,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2">
         <f t="shared" si="1"/>
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="N21" s="2"/>
     </row>
@@ -2909,11 +2909,11 @@
         <v>15</v>
       </c>
       <c r="E22" s="4">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="4">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="4">
@@ -2926,7 +2926,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N22" s="2"/>
     </row>
@@ -2944,11 +2944,11 @@
         <v>48</v>
       </c>
       <c r="E23" s="2">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2">
@@ -2961,7 +2961,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="N23" s="2"/>
     </row>
@@ -3014,11 +3014,11 @@
         <v>16</v>
       </c>
       <c r="E25" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
@@ -3085,17 +3085,17 @@
       </c>
       <c r="E27" s="2">
         <f>SUM(E20:E26)</f>
-        <v>314</v>
+        <v>380</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
         <f>SUM(G20:G26)</f>
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2">
         <f>SUM(I20:I26)</f>
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2">
@@ -3105,7 +3105,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2">
         <f t="shared" si="1"/>
-        <v>1211</v>
+        <v>1244</v>
       </c>
       <c r="N27" s="2"/>
     </row>

</xml_diff>